<commit_message>
update: add new line character check
</commit_message>
<xml_diff>
--- a/members.xlsx
+++ b/members.xlsx
@@ -22,16 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
-    <t xml:space="preserve">会員番号</t>
-  </si>
-  <si>
-    <t xml:space="preserve">氏名</t>
-  </si>
-  <si>
-    <t xml:space="preserve">登録日</t>
-  </si>
-  <si>
-    <t xml:space="preserve">有効期限</t>
+    <t xml:space="preserve">member_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crate_datetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expiration_datetime</t>
   </si>
   <si>
     <t xml:space="preserve">塩見 光洋</t>
@@ -52,7 +52,8 @@
     <t xml:space="preserve">古屋 知世</t>
   </si>
   <si>
-    <t xml:space="preserve">真田 了</t>
+    <t xml:space="preserve">真田 
+ddddd了</t>
   </si>
   <si>
     <t xml:space="preserve">石沢 聡</t>
@@ -174,13 +175,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -203,10 +208,10 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.2734375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14"/>
@@ -311,11 +316,11 @@
         <v>44247</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="30.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>741</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="n">

</xml_diff>